<commit_message>
TC_5-FDR_E2E-FDR-2938-SYSTEM ADMIN REFERENCE DATA
</commit_message>
<xml_diff>
--- a/Data Files/End_2_End/FDR_Create_Voucher.xlsx
+++ b/Data Files/End_2_End/FDR_Create_Voucher.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fdr-automation-develop_08_25_2020\Data Files\End_2_End\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\FDR-Katalon-Regression\Data Files\End_2_End\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAE4711-DE84-43BF-85A1-F6CD147D6405}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409D7A32-9459-49B5-A68A-B9E755134A6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1815" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40695" yWindow="600" windowWidth="13710" windowHeight="10305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FDR_End_End_Reject_TestData" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="167" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -265,14 +265,14 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,12 +556,13 @@
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
@@ -678,11 +679,11 @@
     </row>
     <row r="2" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <v>44104</v>
+        <v>44116</v>
       </c>
       <c r="B2" s="13">
         <f>A2+2</f>
-        <v>44106</v>
+        <v>44118</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>27</v>
@@ -716,19 +717,19 @@
       </c>
       <c r="M2" s="7">
         <f ca="1">TODAY()</f>
-        <v>44092</v>
+        <v>44098</v>
       </c>
       <c r="N2" s="7">
         <f ca="1">TODAY()</f>
-        <v>44092</v>
+        <v>44098</v>
       </c>
       <c r="O2" s="7">
         <f t="shared" ref="O2:P3" ca="1" si="0">TODAY()</f>
-        <v>44092</v>
+        <v>44098</v>
       </c>
       <c r="P2" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>44092</v>
+        <v>44098</v>
       </c>
       <c r="Q2" s="5">
         <v>100000</v>
@@ -769,11 +770,11 @@
     </row>
     <row r="3" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
-        <v>44104</v>
+        <v>44116</v>
       </c>
       <c r="B3" s="13">
         <f>A3+2</f>
-        <v>44106</v>
+        <v>44118</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>27</v>
@@ -807,19 +808,19 @@
       </c>
       <c r="M3" s="7">
         <f ca="1">TODAY()</f>
-        <v>44092</v>
+        <v>44098</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">TODAY()</f>
-        <v>44092</v>
+        <v>44098</v>
       </c>
       <c r="O3" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>44092</v>
+        <v>44098</v>
       </c>
       <c r="P3" s="7">
         <f t="shared" ca="1" si="0"/>
-        <v>44092</v>
+        <v>44098</v>
       </c>
       <c r="Q3" s="5">
         <v>100000</v>

</xml_diff>